<commit_message>
Complete Stories of One City, Thai Cuisine still some problem need to check
</commit_message>
<xml_diff>
--- a/Rasa_basic_folder/Complete_Success_TestCases.xlsx
+++ b/Rasa_basic_folder/Complete_Success_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\Chatbot_GroupProject\Rasa_basic_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5D3E0A8-3CB2-4ED8-AED7-5C5E8E147354}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2340FAC-1117-4B16-8F6E-30A4287ED409}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{77E934E8-2F55-4E53-BC75-7A01658A526A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5070" uniqueCount="117">
   <si>
     <t>ahmedabad</t>
   </si>
@@ -374,15 +374,25 @@
   <si>
     <t>Bot Training Status</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,9 +433,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +889,7 @@
   <dimension ref="A1:E2164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,6 +931,9 @@
       <c r="D2" s="1">
         <v>300</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -934,6 +948,9 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -948,6 +965,9 @@
       <c r="D4" s="1">
         <v>700</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -962,6 +982,9 @@
       <c r="D5" s="1">
         <v>300</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -976,6 +999,9 @@
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -990,6 +1016,9 @@
       <c r="D7" s="1">
         <v>700</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1004,6 +1033,9 @@
       <c r="D8" s="1">
         <v>300</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1018,6 +1050,9 @@
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1032,6 +1067,9 @@
       <c r="D10" s="1">
         <v>700</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1046,6 +1084,9 @@
       <c r="D11" s="1">
         <v>300</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1060,6 +1101,9 @@
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1074,50 +1118,56 @@
       <c r="D13" s="1">
         <v>700</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1">
-        <v>300</v>
-      </c>
+      <c r="D14" s="2">
+        <v>300</v>
+      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="1">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="2">
+        <v>700</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1130,8 +1180,11 @@
       <c r="D17" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,8 +1197,11 @@
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,8 +1214,11 @@
       <c r="D19" s="1">
         <v>700</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,8 +1231,11 @@
       <c r="D20" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1248,11 @@
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,8 +1265,11 @@
       <c r="D22" s="1">
         <v>700</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1283,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1229,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1243,7 +1311,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1257,7 +1325,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1271,7 +1339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1285,7 +1353,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1299,7 +1367,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1395,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -31191,8 +31259,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>